<commit_message>
new data for growth/volume model
</commit_message>
<xml_diff>
--- a/data/sizes/B_2023POGS_small_seed_daily/B_sizes_05132025.xlsx
+++ b/data/sizes/B_2023POGS_small_seed_daily/B_sizes_05132025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graceleuchtenberger/Library/Mobile Documents/com~apple~CloudDocs/Documents/project-gigas-conditioning-GL/data/sizes/B_2023POGS_small_seed_daily/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD37DF73-2153-BB44-AA62-8FC0EC7874FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C725CE30-755F-524C-92A4-ADB46C03E27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="740" windowWidth="24840" windowHeight="17160" xr2:uid="{59562AC7-2699-D84F-A30D-CDAA438C0A0D}"/>
+    <workbookView xWindow="4780" yWindow="1860" windowWidth="24840" windowHeight="17160" xr2:uid="{59562AC7-2699-D84F-A30D-CDAA438C0A0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5016" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5556" uniqueCount="35">
   <si>
     <t>effort</t>
   </si>
@@ -514,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{951AA300-CB28-DA47-A4F6-6DBA5477955B}">
-  <dimension ref="A1:XFD721"/>
+  <dimension ref="A1:XFD811"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A707" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N711" sqref="N711:N721"/>
+      <pane ySplit="1" topLeftCell="A702" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F815" sqref="F815"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36350,6 +36350,3966 @@
         <v>#N/A</v>
       </c>
     </row>
+    <row r="722" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A722" t="s">
+        <v>11</v>
+      </c>
+      <c r="B722" t="s">
+        <v>12</v>
+      </c>
+      <c r="C722" t="s">
+        <v>13</v>
+      </c>
+      <c r="D722" t="s">
+        <v>14</v>
+      </c>
+      <c r="E722" t="s">
+        <v>15</v>
+      </c>
+      <c r="F722" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G722" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H722">
+        <v>8</v>
+      </c>
+      <c r="I722">
+        <v>62</v>
+      </c>
+      <c r="J722" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K722">
+        <v>49.51</v>
+      </c>
+      <c r="L722">
+        <v>39.130000000000003</v>
+      </c>
+      <c r="M722">
+        <v>19.41</v>
+      </c>
+      <c r="N722" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="723" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A723" t="s">
+        <v>11</v>
+      </c>
+      <c r="B723" t="s">
+        <v>12</v>
+      </c>
+      <c r="C723" t="s">
+        <v>13</v>
+      </c>
+      <c r="D723" t="s">
+        <v>14</v>
+      </c>
+      <c r="E723" t="s">
+        <v>15</v>
+      </c>
+      <c r="F723" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G723" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H723">
+        <v>8</v>
+      </c>
+      <c r="I723">
+        <v>62</v>
+      </c>
+      <c r="J723" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K723">
+        <v>75.650000000000006</v>
+      </c>
+      <c r="L723">
+        <v>57.04</v>
+      </c>
+      <c r="M723">
+        <v>21.47</v>
+      </c>
+      <c r="N723" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="724" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A724" t="s">
+        <v>11</v>
+      </c>
+      <c r="B724" t="s">
+        <v>12</v>
+      </c>
+      <c r="C724" t="s">
+        <v>13</v>
+      </c>
+      <c r="D724" t="s">
+        <v>14</v>
+      </c>
+      <c r="E724" t="s">
+        <v>15</v>
+      </c>
+      <c r="F724" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G724" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H724">
+        <v>8</v>
+      </c>
+      <c r="I724">
+        <v>62</v>
+      </c>
+      <c r="J724" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K724">
+        <v>70.489999999999995</v>
+      </c>
+      <c r="L724">
+        <v>46.46</v>
+      </c>
+      <c r="M724">
+        <v>17</v>
+      </c>
+      <c r="N724" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="725" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A725" t="s">
+        <v>11</v>
+      </c>
+      <c r="B725" t="s">
+        <v>12</v>
+      </c>
+      <c r="C725" t="s">
+        <v>13</v>
+      </c>
+      <c r="D725" t="s">
+        <v>14</v>
+      </c>
+      <c r="E725" t="s">
+        <v>15</v>
+      </c>
+      <c r="F725" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G725" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H725">
+        <v>8</v>
+      </c>
+      <c r="I725">
+        <v>62</v>
+      </c>
+      <c r="J725" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K725">
+        <v>53.17</v>
+      </c>
+      <c r="L725">
+        <v>38.76</v>
+      </c>
+      <c r="M725">
+        <v>21.1</v>
+      </c>
+      <c r="N725" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="726" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A726" t="s">
+        <v>11</v>
+      </c>
+      <c r="B726" t="s">
+        <v>12</v>
+      </c>
+      <c r="C726" t="s">
+        <v>13</v>
+      </c>
+      <c r="D726" t="s">
+        <v>14</v>
+      </c>
+      <c r="E726" t="s">
+        <v>15</v>
+      </c>
+      <c r="F726" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G726" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H726">
+        <v>8</v>
+      </c>
+      <c r="I726">
+        <v>62</v>
+      </c>
+      <c r="J726" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K726">
+        <v>65.53</v>
+      </c>
+      <c r="L726">
+        <v>38.31</v>
+      </c>
+      <c r="M726">
+        <v>15.78</v>
+      </c>
+      <c r="N726" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="727" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A727" t="s">
+        <v>11</v>
+      </c>
+      <c r="B727" t="s">
+        <v>12</v>
+      </c>
+      <c r="C727" t="s">
+        <v>13</v>
+      </c>
+      <c r="D727" t="s">
+        <v>14</v>
+      </c>
+      <c r="E727" t="s">
+        <v>15</v>
+      </c>
+      <c r="F727" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G727" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H727">
+        <v>8</v>
+      </c>
+      <c r="I727">
+        <v>62</v>
+      </c>
+      <c r="J727" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K727">
+        <v>56.37</v>
+      </c>
+      <c r="L727">
+        <v>35.619999999999997</v>
+      </c>
+      <c r="M727">
+        <v>14.03</v>
+      </c>
+      <c r="N727" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="728" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A728" t="s">
+        <v>11</v>
+      </c>
+      <c r="B728" t="s">
+        <v>12</v>
+      </c>
+      <c r="C728" t="s">
+        <v>13</v>
+      </c>
+      <c r="D728" t="s">
+        <v>14</v>
+      </c>
+      <c r="E728" t="s">
+        <v>15</v>
+      </c>
+      <c r="F728" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G728" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H728">
+        <v>8</v>
+      </c>
+      <c r="I728">
+        <v>62</v>
+      </c>
+      <c r="J728" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K728">
+        <v>74.22</v>
+      </c>
+      <c r="L728">
+        <v>45.2</v>
+      </c>
+      <c r="M728">
+        <v>17.22</v>
+      </c>
+      <c r="N728" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="729" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A729" t="s">
+        <v>11</v>
+      </c>
+      <c r="B729" t="s">
+        <v>12</v>
+      </c>
+      <c r="C729" t="s">
+        <v>13</v>
+      </c>
+      <c r="D729" t="s">
+        <v>14</v>
+      </c>
+      <c r="E729" t="s">
+        <v>15</v>
+      </c>
+      <c r="F729" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G729" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H729">
+        <v>8</v>
+      </c>
+      <c r="I729">
+        <v>62</v>
+      </c>
+      <c r="J729" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K729">
+        <v>67.709999999999994</v>
+      </c>
+      <c r="L729">
+        <v>54.22</v>
+      </c>
+      <c r="M729">
+        <v>20.6</v>
+      </c>
+      <c r="N729" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="730" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A730" t="s">
+        <v>11</v>
+      </c>
+      <c r="B730" t="s">
+        <v>12</v>
+      </c>
+      <c r="C730" t="s">
+        <v>13</v>
+      </c>
+      <c r="D730" t="s">
+        <v>14</v>
+      </c>
+      <c r="E730" t="s">
+        <v>15</v>
+      </c>
+      <c r="F730" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G730" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H730">
+        <v>8</v>
+      </c>
+      <c r="I730">
+        <v>62</v>
+      </c>
+      <c r="J730" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K730">
+        <v>53.19</v>
+      </c>
+      <c r="L730">
+        <v>30.57</v>
+      </c>
+      <c r="M730">
+        <v>16.5</v>
+      </c>
+      <c r="N730" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="731" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A731" t="s">
+        <v>11</v>
+      </c>
+      <c r="B731" t="s">
+        <v>12</v>
+      </c>
+      <c r="C731" t="s">
+        <v>13</v>
+      </c>
+      <c r="D731" t="s">
+        <v>14</v>
+      </c>
+      <c r="E731" t="s">
+        <v>15</v>
+      </c>
+      <c r="F731" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G731" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H731">
+        <v>8</v>
+      </c>
+      <c r="I731">
+        <v>62</v>
+      </c>
+      <c r="J731" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K731">
+        <v>51.42</v>
+      </c>
+      <c r="L731">
+        <v>37.619999999999997</v>
+      </c>
+      <c r="M731">
+        <v>16.21</v>
+      </c>
+      <c r="N731" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="732" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A732" t="s">
+        <v>11</v>
+      </c>
+      <c r="B732" t="s">
+        <v>12</v>
+      </c>
+      <c r="C732" t="s">
+        <v>13</v>
+      </c>
+      <c r="D732" t="s">
+        <v>16</v>
+      </c>
+      <c r="E732" t="s">
+        <v>15</v>
+      </c>
+      <c r="F732" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G732" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H732">
+        <v>5</v>
+      </c>
+      <c r="I732">
+        <v>73</v>
+      </c>
+      <c r="J732" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K732">
+        <v>85.86</v>
+      </c>
+      <c r="L732">
+        <v>49.02</v>
+      </c>
+      <c r="M732">
+        <v>21.08</v>
+      </c>
+      <c r="N732" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="733" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A733" t="s">
+        <v>11</v>
+      </c>
+      <c r="B733" t="s">
+        <v>12</v>
+      </c>
+      <c r="C733" t="s">
+        <v>13</v>
+      </c>
+      <c r="D733" t="s">
+        <v>16</v>
+      </c>
+      <c r="E733" t="s">
+        <v>15</v>
+      </c>
+      <c r="F733" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G733" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H733">
+        <v>5</v>
+      </c>
+      <c r="I733">
+        <v>73</v>
+      </c>
+      <c r="J733" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K733">
+        <v>65.95</v>
+      </c>
+      <c r="L733">
+        <v>40.19</v>
+      </c>
+      <c r="M733">
+        <v>17.23</v>
+      </c>
+      <c r="N733" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="734" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A734" t="s">
+        <v>11</v>
+      </c>
+      <c r="B734" t="s">
+        <v>12</v>
+      </c>
+      <c r="C734" t="s">
+        <v>13</v>
+      </c>
+      <c r="D734" t="s">
+        <v>16</v>
+      </c>
+      <c r="E734" t="s">
+        <v>15</v>
+      </c>
+      <c r="F734" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G734" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H734">
+        <v>5</v>
+      </c>
+      <c r="I734">
+        <v>73</v>
+      </c>
+      <c r="J734" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K734">
+        <v>62.96</v>
+      </c>
+      <c r="L734">
+        <v>47.35</v>
+      </c>
+      <c r="M734">
+        <v>15.57</v>
+      </c>
+      <c r="N734" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="735" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A735" t="s">
+        <v>11</v>
+      </c>
+      <c r="B735" t="s">
+        <v>12</v>
+      </c>
+      <c r="C735" t="s">
+        <v>13</v>
+      </c>
+      <c r="D735" t="s">
+        <v>16</v>
+      </c>
+      <c r="E735" t="s">
+        <v>15</v>
+      </c>
+      <c r="F735" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G735" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H735">
+        <v>5</v>
+      </c>
+      <c r="I735">
+        <v>73</v>
+      </c>
+      <c r="J735" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K735">
+        <v>47.49</v>
+      </c>
+      <c r="L735">
+        <v>37.159999999999997</v>
+      </c>
+      <c r="M735">
+        <v>15.35</v>
+      </c>
+      <c r="N735" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="736" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A736" t="s">
+        <v>11</v>
+      </c>
+      <c r="B736" t="s">
+        <v>12</v>
+      </c>
+      <c r="C736" t="s">
+        <v>13</v>
+      </c>
+      <c r="D736" t="s">
+        <v>16</v>
+      </c>
+      <c r="E736" t="s">
+        <v>15</v>
+      </c>
+      <c r="F736" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G736" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H736">
+        <v>5</v>
+      </c>
+      <c r="I736">
+        <v>73</v>
+      </c>
+      <c r="J736" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K736">
+        <v>57.27</v>
+      </c>
+      <c r="L736">
+        <v>35.99</v>
+      </c>
+      <c r="M736">
+        <v>21.79</v>
+      </c>
+      <c r="N736" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="737" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A737" t="s">
+        <v>11</v>
+      </c>
+      <c r="B737" t="s">
+        <v>12</v>
+      </c>
+      <c r="C737" t="s">
+        <v>13</v>
+      </c>
+      <c r="D737" t="s">
+        <v>16</v>
+      </c>
+      <c r="E737" t="s">
+        <v>15</v>
+      </c>
+      <c r="F737" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G737" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H737">
+        <v>5</v>
+      </c>
+      <c r="I737">
+        <v>73</v>
+      </c>
+      <c r="J737" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K737">
+        <v>32.21</v>
+      </c>
+      <c r="L737">
+        <v>37.94</v>
+      </c>
+      <c r="M737">
+        <v>13.41</v>
+      </c>
+      <c r="N737" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="738" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A738" t="s">
+        <v>11</v>
+      </c>
+      <c r="B738" t="s">
+        <v>12</v>
+      </c>
+      <c r="C738" t="s">
+        <v>13</v>
+      </c>
+      <c r="D738" t="s">
+        <v>16</v>
+      </c>
+      <c r="E738" t="s">
+        <v>15</v>
+      </c>
+      <c r="F738" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G738" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H738">
+        <v>5</v>
+      </c>
+      <c r="I738">
+        <v>73</v>
+      </c>
+      <c r="J738" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K738">
+        <v>74.28</v>
+      </c>
+      <c r="L738">
+        <v>51.28</v>
+      </c>
+      <c r="M738">
+        <v>19.43</v>
+      </c>
+      <c r="N738" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="739" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A739" t="s">
+        <v>11</v>
+      </c>
+      <c r="B739" t="s">
+        <v>12</v>
+      </c>
+      <c r="C739" t="s">
+        <v>13</v>
+      </c>
+      <c r="D739" t="s">
+        <v>16</v>
+      </c>
+      <c r="E739" t="s">
+        <v>15</v>
+      </c>
+      <c r="F739" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G739" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H739">
+        <v>5</v>
+      </c>
+      <c r="I739">
+        <v>73</v>
+      </c>
+      <c r="J739" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K739">
+        <v>80.14</v>
+      </c>
+      <c r="L739">
+        <v>49.9</v>
+      </c>
+      <c r="M739">
+        <v>22.98</v>
+      </c>
+      <c r="N739" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="740" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A740" t="s">
+        <v>11</v>
+      </c>
+      <c r="B740" t="s">
+        <v>12</v>
+      </c>
+      <c r="C740" t="s">
+        <v>13</v>
+      </c>
+      <c r="D740" t="s">
+        <v>16</v>
+      </c>
+      <c r="E740" t="s">
+        <v>15</v>
+      </c>
+      <c r="F740" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G740" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H740">
+        <v>5</v>
+      </c>
+      <c r="I740">
+        <v>73</v>
+      </c>
+      <c r="J740" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K740">
+        <v>68.75</v>
+      </c>
+      <c r="L740">
+        <v>38.49</v>
+      </c>
+      <c r="M740">
+        <v>19.88</v>
+      </c>
+      <c r="N740" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="741" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A741" t="s">
+        <v>11</v>
+      </c>
+      <c r="B741" t="s">
+        <v>12</v>
+      </c>
+      <c r="C741" t="s">
+        <v>13</v>
+      </c>
+      <c r="D741" t="s">
+        <v>16</v>
+      </c>
+      <c r="E741" t="s">
+        <v>15</v>
+      </c>
+      <c r="F741" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G741" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H741">
+        <v>5</v>
+      </c>
+      <c r="I741">
+        <v>73</v>
+      </c>
+      <c r="J741" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K741">
+        <v>56.98</v>
+      </c>
+      <c r="L741">
+        <v>41.84</v>
+      </c>
+      <c r="M741">
+        <v>18.8</v>
+      </c>
+      <c r="N741" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="742" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A742" t="s">
+        <v>11</v>
+      </c>
+      <c r="B742" t="s">
+        <v>12</v>
+      </c>
+      <c r="C742" t="s">
+        <v>13</v>
+      </c>
+      <c r="D742" t="s">
+        <v>14</v>
+      </c>
+      <c r="E742" t="s">
+        <v>15</v>
+      </c>
+      <c r="F742" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G742" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H742">
+        <v>10</v>
+      </c>
+      <c r="I742">
+        <v>72</v>
+      </c>
+      <c r="J742" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K742">
+        <v>50.36</v>
+      </c>
+      <c r="L742">
+        <v>40.93</v>
+      </c>
+      <c r="M742">
+        <v>17.05</v>
+      </c>
+      <c r="N742" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="743" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A743" t="s">
+        <v>11</v>
+      </c>
+      <c r="B743" t="s">
+        <v>12</v>
+      </c>
+      <c r="C743" t="s">
+        <v>13</v>
+      </c>
+      <c r="D743" t="s">
+        <v>14</v>
+      </c>
+      <c r="E743" t="s">
+        <v>15</v>
+      </c>
+      <c r="F743" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G743" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H743">
+        <v>10</v>
+      </c>
+      <c r="I743">
+        <v>72</v>
+      </c>
+      <c r="J743" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K743">
+        <v>44.85</v>
+      </c>
+      <c r="L743">
+        <v>33.119999999999997</v>
+      </c>
+      <c r="M743">
+        <v>13.67</v>
+      </c>
+      <c r="N743" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="744" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A744" t="s">
+        <v>11</v>
+      </c>
+      <c r="B744" t="s">
+        <v>12</v>
+      </c>
+      <c r="C744" t="s">
+        <v>13</v>
+      </c>
+      <c r="D744" t="s">
+        <v>14</v>
+      </c>
+      <c r="E744" t="s">
+        <v>15</v>
+      </c>
+      <c r="F744" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G744" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H744">
+        <v>10</v>
+      </c>
+      <c r="I744">
+        <v>72</v>
+      </c>
+      <c r="J744" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K744">
+        <v>49.04</v>
+      </c>
+      <c r="L744">
+        <v>35.31</v>
+      </c>
+      <c r="M744">
+        <v>13.41</v>
+      </c>
+      <c r="N744" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="745" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A745" t="s">
+        <v>11</v>
+      </c>
+      <c r="B745" t="s">
+        <v>12</v>
+      </c>
+      <c r="C745" t="s">
+        <v>13</v>
+      </c>
+      <c r="D745" t="s">
+        <v>14</v>
+      </c>
+      <c r="E745" t="s">
+        <v>15</v>
+      </c>
+      <c r="F745" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G745" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H745">
+        <v>10</v>
+      </c>
+      <c r="I745">
+        <v>72</v>
+      </c>
+      <c r="J745" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K745">
+        <v>72.06</v>
+      </c>
+      <c r="L745">
+        <v>51.9</v>
+      </c>
+      <c r="M745">
+        <v>20.420000000000002</v>
+      </c>
+      <c r="N745" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="746" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A746" t="s">
+        <v>11</v>
+      </c>
+      <c r="B746" t="s">
+        <v>12</v>
+      </c>
+      <c r="C746" t="s">
+        <v>13</v>
+      </c>
+      <c r="D746" t="s">
+        <v>14</v>
+      </c>
+      <c r="E746" t="s">
+        <v>15</v>
+      </c>
+      <c r="F746" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G746" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H746">
+        <v>10</v>
+      </c>
+      <c r="I746">
+        <v>72</v>
+      </c>
+      <c r="J746" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K746">
+        <v>74.02</v>
+      </c>
+      <c r="L746">
+        <v>42.04</v>
+      </c>
+      <c r="M746">
+        <v>21</v>
+      </c>
+      <c r="N746" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="747" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A747" t="s">
+        <v>11</v>
+      </c>
+      <c r="B747" t="s">
+        <v>12</v>
+      </c>
+      <c r="C747" t="s">
+        <v>13</v>
+      </c>
+      <c r="D747" t="s">
+        <v>14</v>
+      </c>
+      <c r="E747" t="s">
+        <v>15</v>
+      </c>
+      <c r="F747" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G747" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H747">
+        <v>10</v>
+      </c>
+      <c r="I747">
+        <v>72</v>
+      </c>
+      <c r="J747" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K747">
+        <v>58.77</v>
+      </c>
+      <c r="L747">
+        <v>40.81</v>
+      </c>
+      <c r="M747">
+        <v>19.66</v>
+      </c>
+      <c r="N747" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="748" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A748" t="s">
+        <v>11</v>
+      </c>
+      <c r="B748" t="s">
+        <v>12</v>
+      </c>
+      <c r="C748" t="s">
+        <v>13</v>
+      </c>
+      <c r="D748" t="s">
+        <v>14</v>
+      </c>
+      <c r="E748" t="s">
+        <v>15</v>
+      </c>
+      <c r="F748" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G748" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H748">
+        <v>10</v>
+      </c>
+      <c r="I748">
+        <v>72</v>
+      </c>
+      <c r="J748" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K748">
+        <v>53.47</v>
+      </c>
+      <c r="L748">
+        <v>41.27</v>
+      </c>
+      <c r="M748">
+        <v>15.39</v>
+      </c>
+      <c r="N748" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="749" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A749" t="s">
+        <v>11</v>
+      </c>
+      <c r="B749" t="s">
+        <v>12</v>
+      </c>
+      <c r="C749" t="s">
+        <v>13</v>
+      </c>
+      <c r="D749" t="s">
+        <v>14</v>
+      </c>
+      <c r="E749" t="s">
+        <v>15</v>
+      </c>
+      <c r="F749" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G749" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H749">
+        <v>10</v>
+      </c>
+      <c r="I749">
+        <v>72</v>
+      </c>
+      <c r="J749" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K749">
+        <v>44.16</v>
+      </c>
+      <c r="L749">
+        <v>34.44</v>
+      </c>
+      <c r="M749">
+        <v>15.49</v>
+      </c>
+      <c r="N749" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="750" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A750" t="s">
+        <v>11</v>
+      </c>
+      <c r="B750" t="s">
+        <v>12</v>
+      </c>
+      <c r="C750" t="s">
+        <v>13</v>
+      </c>
+      <c r="D750" t="s">
+        <v>14</v>
+      </c>
+      <c r="E750" t="s">
+        <v>15</v>
+      </c>
+      <c r="F750" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G750" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H750">
+        <v>10</v>
+      </c>
+      <c r="I750">
+        <v>72</v>
+      </c>
+      <c r="J750" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K750">
+        <v>55.83</v>
+      </c>
+      <c r="L750">
+        <v>34.54</v>
+      </c>
+      <c r="M750">
+        <v>18.38</v>
+      </c>
+      <c r="N750" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="751" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A751" t="s">
+        <v>11</v>
+      </c>
+      <c r="B751" t="s">
+        <v>12</v>
+      </c>
+      <c r="C751" t="s">
+        <v>13</v>
+      </c>
+      <c r="D751" t="s">
+        <v>14</v>
+      </c>
+      <c r="E751" t="s">
+        <v>15</v>
+      </c>
+      <c r="F751" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G751" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H751">
+        <v>10</v>
+      </c>
+      <c r="I751">
+        <v>72</v>
+      </c>
+      <c r="J751" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K751">
+        <v>82.53</v>
+      </c>
+      <c r="L751">
+        <v>58.46</v>
+      </c>
+      <c r="M751">
+        <v>22.72</v>
+      </c>
+      <c r="N751" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="752" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A752" t="s">
+        <v>11</v>
+      </c>
+      <c r="B752" t="s">
+        <v>12</v>
+      </c>
+      <c r="C752" t="s">
+        <v>13</v>
+      </c>
+      <c r="D752" t="s">
+        <v>14</v>
+      </c>
+      <c r="E752" t="s">
+        <v>15</v>
+      </c>
+      <c r="F752" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G752" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H752">
+        <v>6</v>
+      </c>
+      <c r="I752">
+        <v>67</v>
+      </c>
+      <c r="J752" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K752">
+        <v>42.86</v>
+      </c>
+      <c r="L752">
+        <v>29.35</v>
+      </c>
+      <c r="M752">
+        <v>13.19</v>
+      </c>
+      <c r="N752" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="753" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A753" t="s">
+        <v>11</v>
+      </c>
+      <c r="B753" t="s">
+        <v>12</v>
+      </c>
+      <c r="C753" t="s">
+        <v>13</v>
+      </c>
+      <c r="D753" t="s">
+        <v>14</v>
+      </c>
+      <c r="E753" t="s">
+        <v>15</v>
+      </c>
+      <c r="F753" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G753" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H753">
+        <v>6</v>
+      </c>
+      <c r="I753">
+        <v>67</v>
+      </c>
+      <c r="J753" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K753">
+        <v>42.97</v>
+      </c>
+      <c r="L753">
+        <v>35.97</v>
+      </c>
+      <c r="M753">
+        <v>12.53</v>
+      </c>
+      <c r="N753" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="754" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A754" t="s">
+        <v>11</v>
+      </c>
+      <c r="B754" t="s">
+        <v>12</v>
+      </c>
+      <c r="C754" t="s">
+        <v>13</v>
+      </c>
+      <c r="D754" t="s">
+        <v>14</v>
+      </c>
+      <c r="E754" t="s">
+        <v>15</v>
+      </c>
+      <c r="F754" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G754" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H754">
+        <v>6</v>
+      </c>
+      <c r="I754">
+        <v>67</v>
+      </c>
+      <c r="J754" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K754">
+        <v>54.59</v>
+      </c>
+      <c r="L754">
+        <v>43.9</v>
+      </c>
+      <c r="M754">
+        <v>20.9</v>
+      </c>
+      <c r="N754" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="755" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A755" t="s">
+        <v>11</v>
+      </c>
+      <c r="B755" t="s">
+        <v>12</v>
+      </c>
+      <c r="C755" t="s">
+        <v>13</v>
+      </c>
+      <c r="D755" t="s">
+        <v>14</v>
+      </c>
+      <c r="E755" t="s">
+        <v>15</v>
+      </c>
+      <c r="F755" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G755" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H755">
+        <v>6</v>
+      </c>
+      <c r="I755">
+        <v>67</v>
+      </c>
+      <c r="J755" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K755">
+        <v>76.12</v>
+      </c>
+      <c r="L755">
+        <v>51.7</v>
+      </c>
+      <c r="M755">
+        <v>18.45</v>
+      </c>
+      <c r="N755" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="756" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A756" t="s">
+        <v>11</v>
+      </c>
+      <c r="B756" t="s">
+        <v>12</v>
+      </c>
+      <c r="C756" t="s">
+        <v>13</v>
+      </c>
+      <c r="D756" t="s">
+        <v>14</v>
+      </c>
+      <c r="E756" t="s">
+        <v>15</v>
+      </c>
+      <c r="F756" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G756" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H756">
+        <v>6</v>
+      </c>
+      <c r="I756">
+        <v>67</v>
+      </c>
+      <c r="J756" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K756">
+        <v>53.33</v>
+      </c>
+      <c r="L756">
+        <v>39.520000000000003</v>
+      </c>
+      <c r="M756">
+        <v>15.23</v>
+      </c>
+      <c r="N756" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="757" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A757" t="s">
+        <v>11</v>
+      </c>
+      <c r="B757" t="s">
+        <v>12</v>
+      </c>
+      <c r="C757" t="s">
+        <v>13</v>
+      </c>
+      <c r="D757" t="s">
+        <v>14</v>
+      </c>
+      <c r="E757" t="s">
+        <v>15</v>
+      </c>
+      <c r="F757" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G757" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H757">
+        <v>6</v>
+      </c>
+      <c r="I757">
+        <v>67</v>
+      </c>
+      <c r="J757" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K757">
+        <v>67.88</v>
+      </c>
+      <c r="L757">
+        <v>39.479999999999997</v>
+      </c>
+      <c r="M757">
+        <v>24.95</v>
+      </c>
+      <c r="N757" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="758" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A758" t="s">
+        <v>11</v>
+      </c>
+      <c r="B758" t="s">
+        <v>12</v>
+      </c>
+      <c r="C758" t="s">
+        <v>13</v>
+      </c>
+      <c r="D758" t="s">
+        <v>14</v>
+      </c>
+      <c r="E758" t="s">
+        <v>15</v>
+      </c>
+      <c r="F758" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G758" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H758">
+        <v>6</v>
+      </c>
+      <c r="I758">
+        <v>67</v>
+      </c>
+      <c r="J758" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K758">
+        <v>50.15</v>
+      </c>
+      <c r="L758">
+        <v>41.07</v>
+      </c>
+      <c r="M758">
+        <v>16.04</v>
+      </c>
+      <c r="N758" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="759" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A759" t="s">
+        <v>11</v>
+      </c>
+      <c r="B759" t="s">
+        <v>12</v>
+      </c>
+      <c r="C759" t="s">
+        <v>13</v>
+      </c>
+      <c r="D759" t="s">
+        <v>14</v>
+      </c>
+      <c r="E759" t="s">
+        <v>15</v>
+      </c>
+      <c r="F759" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G759" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H759">
+        <v>6</v>
+      </c>
+      <c r="I759">
+        <v>67</v>
+      </c>
+      <c r="J759" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K759">
+        <v>51</v>
+      </c>
+      <c r="L759">
+        <v>44.76</v>
+      </c>
+      <c r="M759">
+        <v>12.85</v>
+      </c>
+      <c r="N759" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="760" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A760" t="s">
+        <v>11</v>
+      </c>
+      <c r="B760" t="s">
+        <v>12</v>
+      </c>
+      <c r="C760" t="s">
+        <v>13</v>
+      </c>
+      <c r="D760" t="s">
+        <v>14</v>
+      </c>
+      <c r="E760" t="s">
+        <v>15</v>
+      </c>
+      <c r="F760" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G760" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H760">
+        <v>6</v>
+      </c>
+      <c r="I760">
+        <v>67</v>
+      </c>
+      <c r="J760" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K760">
+        <v>51.52</v>
+      </c>
+      <c r="L760">
+        <v>52.75</v>
+      </c>
+      <c r="M760">
+        <v>18.260000000000002</v>
+      </c>
+      <c r="N760" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="761" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A761" t="s">
+        <v>11</v>
+      </c>
+      <c r="B761" t="s">
+        <v>12</v>
+      </c>
+      <c r="C761" t="s">
+        <v>13</v>
+      </c>
+      <c r="D761" t="s">
+        <v>14</v>
+      </c>
+      <c r="E761" t="s">
+        <v>15</v>
+      </c>
+      <c r="F761" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G761" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H761">
+        <v>6</v>
+      </c>
+      <c r="I761">
+        <v>67</v>
+      </c>
+      <c r="J761" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K761">
+        <v>64.06</v>
+      </c>
+      <c r="L761">
+        <v>51.22</v>
+      </c>
+      <c r="M761">
+        <v>24.31</v>
+      </c>
+      <c r="N761" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="762" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A762" t="s">
+        <v>11</v>
+      </c>
+      <c r="B762" t="s">
+        <v>12</v>
+      </c>
+      <c r="C762" t="s">
+        <v>13</v>
+      </c>
+      <c r="D762" t="s">
+        <v>16</v>
+      </c>
+      <c r="E762" t="s">
+        <v>15</v>
+      </c>
+      <c r="F762" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G762" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H762">
+        <v>1</v>
+      </c>
+      <c r="I762">
+        <v>53</v>
+      </c>
+      <c r="J762" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K762">
+        <v>48.58</v>
+      </c>
+      <c r="L762">
+        <v>40.880000000000003</v>
+      </c>
+      <c r="M762">
+        <v>15.22</v>
+      </c>
+      <c r="N762" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="763" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A763" t="s">
+        <v>11</v>
+      </c>
+      <c r="B763" t="s">
+        <v>12</v>
+      </c>
+      <c r="C763" t="s">
+        <v>13</v>
+      </c>
+      <c r="D763" t="s">
+        <v>16</v>
+      </c>
+      <c r="E763" t="s">
+        <v>15</v>
+      </c>
+      <c r="F763" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G763" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H763">
+        <v>1</v>
+      </c>
+      <c r="I763">
+        <v>53</v>
+      </c>
+      <c r="J763" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K763">
+        <v>50.54</v>
+      </c>
+      <c r="L763">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="M763">
+        <v>14.36</v>
+      </c>
+      <c r="N763" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="764" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A764" t="s">
+        <v>11</v>
+      </c>
+      <c r="B764" t="s">
+        <v>12</v>
+      </c>
+      <c r="C764" t="s">
+        <v>13</v>
+      </c>
+      <c r="D764" t="s">
+        <v>16</v>
+      </c>
+      <c r="E764" t="s">
+        <v>15</v>
+      </c>
+      <c r="F764" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G764" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H764">
+        <v>1</v>
+      </c>
+      <c r="I764">
+        <v>53</v>
+      </c>
+      <c r="J764" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K764">
+        <v>54.77</v>
+      </c>
+      <c r="L764">
+        <v>43.98</v>
+      </c>
+      <c r="M764">
+        <v>15.18</v>
+      </c>
+      <c r="N764" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="765" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A765" t="s">
+        <v>11</v>
+      </c>
+      <c r="B765" t="s">
+        <v>12</v>
+      </c>
+      <c r="C765" t="s">
+        <v>13</v>
+      </c>
+      <c r="D765" t="s">
+        <v>16</v>
+      </c>
+      <c r="E765" t="s">
+        <v>15</v>
+      </c>
+      <c r="F765" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G765" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H765">
+        <v>1</v>
+      </c>
+      <c r="I765">
+        <v>53</v>
+      </c>
+      <c r="J765" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K765">
+        <v>65</v>
+      </c>
+      <c r="L765">
+        <v>37.159999999999997</v>
+      </c>
+      <c r="M765">
+        <v>19.46</v>
+      </c>
+      <c r="N765" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="766" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A766" t="s">
+        <v>11</v>
+      </c>
+      <c r="B766" t="s">
+        <v>12</v>
+      </c>
+      <c r="C766" t="s">
+        <v>13</v>
+      </c>
+      <c r="D766" t="s">
+        <v>16</v>
+      </c>
+      <c r="E766" t="s">
+        <v>15</v>
+      </c>
+      <c r="F766" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G766" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H766">
+        <v>1</v>
+      </c>
+      <c r="I766">
+        <v>53</v>
+      </c>
+      <c r="J766" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K766">
+        <v>49.26</v>
+      </c>
+      <c r="L766">
+        <v>37.93</v>
+      </c>
+      <c r="M766">
+        <v>15.96</v>
+      </c>
+      <c r="N766" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="767" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A767" t="s">
+        <v>11</v>
+      </c>
+      <c r="B767" t="s">
+        <v>12</v>
+      </c>
+      <c r="C767" t="s">
+        <v>13</v>
+      </c>
+      <c r="D767" t="s">
+        <v>16</v>
+      </c>
+      <c r="E767" t="s">
+        <v>15</v>
+      </c>
+      <c r="F767" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G767" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H767">
+        <v>1</v>
+      </c>
+      <c r="I767">
+        <v>53</v>
+      </c>
+      <c r="J767" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K767">
+        <v>61.28</v>
+      </c>
+      <c r="L767">
+        <v>45.51</v>
+      </c>
+      <c r="M767">
+        <v>20.67</v>
+      </c>
+      <c r="N767" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="768" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A768" t="s">
+        <v>11</v>
+      </c>
+      <c r="B768" t="s">
+        <v>12</v>
+      </c>
+      <c r="C768" t="s">
+        <v>13</v>
+      </c>
+      <c r="D768" t="s">
+        <v>16</v>
+      </c>
+      <c r="E768" t="s">
+        <v>15</v>
+      </c>
+      <c r="F768" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G768" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H768">
+        <v>1</v>
+      </c>
+      <c r="I768">
+        <v>53</v>
+      </c>
+      <c r="J768" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K768">
+        <v>69.12</v>
+      </c>
+      <c r="L768">
+        <v>43.57</v>
+      </c>
+      <c r="M768">
+        <v>15.33</v>
+      </c>
+      <c r="N768" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="769" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A769" t="s">
+        <v>11</v>
+      </c>
+      <c r="B769" t="s">
+        <v>12</v>
+      </c>
+      <c r="C769" t="s">
+        <v>13</v>
+      </c>
+      <c r="D769" t="s">
+        <v>16</v>
+      </c>
+      <c r="E769" t="s">
+        <v>15</v>
+      </c>
+      <c r="F769" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G769" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H769">
+        <v>1</v>
+      </c>
+      <c r="I769">
+        <v>53</v>
+      </c>
+      <c r="J769" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K769">
+        <v>67.59</v>
+      </c>
+      <c r="L769">
+        <v>55.55</v>
+      </c>
+      <c r="M769">
+        <v>20.2</v>
+      </c>
+      <c r="N769" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="770" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A770" t="s">
+        <v>11</v>
+      </c>
+      <c r="B770" t="s">
+        <v>12</v>
+      </c>
+      <c r="C770" t="s">
+        <v>13</v>
+      </c>
+      <c r="D770" t="s">
+        <v>16</v>
+      </c>
+      <c r="E770" t="s">
+        <v>15</v>
+      </c>
+      <c r="F770" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G770" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H770">
+        <v>1</v>
+      </c>
+      <c r="I770">
+        <v>53</v>
+      </c>
+      <c r="J770" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K770">
+        <v>54.9</v>
+      </c>
+      <c r="L770">
+        <v>42.28</v>
+      </c>
+      <c r="M770">
+        <v>21.33</v>
+      </c>
+      <c r="N770" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="771" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A771" t="s">
+        <v>11</v>
+      </c>
+      <c r="B771" t="s">
+        <v>12</v>
+      </c>
+      <c r="C771" t="s">
+        <v>13</v>
+      </c>
+      <c r="D771" t="s">
+        <v>16</v>
+      </c>
+      <c r="E771" t="s">
+        <v>15</v>
+      </c>
+      <c r="F771" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G771" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H771">
+        <v>1</v>
+      </c>
+      <c r="I771">
+        <v>53</v>
+      </c>
+      <c r="J771" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K771">
+        <v>52.73</v>
+      </c>
+      <c r="L771">
+        <v>42.32</v>
+      </c>
+      <c r="M771">
+        <v>15.2</v>
+      </c>
+      <c r="N771" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="772" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A772" t="s">
+        <v>11</v>
+      </c>
+      <c r="B772" t="s">
+        <v>12</v>
+      </c>
+      <c r="C772" t="s">
+        <v>13</v>
+      </c>
+      <c r="D772" t="s">
+        <v>16</v>
+      </c>
+      <c r="E772" t="s">
+        <v>15</v>
+      </c>
+      <c r="F772" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G772" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H772">
+        <v>2</v>
+      </c>
+      <c r="I772">
+        <v>78</v>
+      </c>
+      <c r="J772" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K772">
+        <v>40.82</v>
+      </c>
+      <c r="L772">
+        <v>29.84</v>
+      </c>
+      <c r="M772">
+        <v>19.43</v>
+      </c>
+      <c r="N772" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="773" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A773" t="s">
+        <v>11</v>
+      </c>
+      <c r="B773" t="s">
+        <v>12</v>
+      </c>
+      <c r="C773" t="s">
+        <v>13</v>
+      </c>
+      <c r="D773" t="s">
+        <v>16</v>
+      </c>
+      <c r="E773" t="s">
+        <v>15</v>
+      </c>
+      <c r="F773" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G773" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H773">
+        <v>2</v>
+      </c>
+      <c r="I773">
+        <v>78</v>
+      </c>
+      <c r="J773" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K773">
+        <v>51.25</v>
+      </c>
+      <c r="L773">
+        <v>33.159999999999997</v>
+      </c>
+      <c r="M773">
+        <v>13.84</v>
+      </c>
+      <c r="N773" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="774" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A774" t="s">
+        <v>11</v>
+      </c>
+      <c r="B774" t="s">
+        <v>12</v>
+      </c>
+      <c r="C774" t="s">
+        <v>13</v>
+      </c>
+      <c r="D774" t="s">
+        <v>16</v>
+      </c>
+      <c r="E774" t="s">
+        <v>15</v>
+      </c>
+      <c r="F774" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G774" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H774">
+        <v>2</v>
+      </c>
+      <c r="I774">
+        <v>78</v>
+      </c>
+      <c r="J774" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K774">
+        <v>65.2</v>
+      </c>
+      <c r="L774">
+        <v>39.74</v>
+      </c>
+      <c r="M774">
+        <v>18.45</v>
+      </c>
+      <c r="N774" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="775" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A775" t="s">
+        <v>11</v>
+      </c>
+      <c r="B775" t="s">
+        <v>12</v>
+      </c>
+      <c r="C775" t="s">
+        <v>13</v>
+      </c>
+      <c r="D775" t="s">
+        <v>16</v>
+      </c>
+      <c r="E775" t="s">
+        <v>15</v>
+      </c>
+      <c r="F775" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G775" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H775">
+        <v>2</v>
+      </c>
+      <c r="I775">
+        <v>78</v>
+      </c>
+      <c r="J775" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K775">
+        <v>48.98</v>
+      </c>
+      <c r="L775">
+        <v>24.19</v>
+      </c>
+      <c r="M775">
+        <v>15.29</v>
+      </c>
+      <c r="N775" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="776" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A776" t="s">
+        <v>11</v>
+      </c>
+      <c r="B776" t="s">
+        <v>12</v>
+      </c>
+      <c r="C776" t="s">
+        <v>13</v>
+      </c>
+      <c r="D776" t="s">
+        <v>16</v>
+      </c>
+      <c r="E776" t="s">
+        <v>15</v>
+      </c>
+      <c r="F776" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G776" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H776">
+        <v>2</v>
+      </c>
+      <c r="I776">
+        <v>78</v>
+      </c>
+      <c r="J776" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K776">
+        <v>51.32</v>
+      </c>
+      <c r="L776">
+        <v>39.61</v>
+      </c>
+      <c r="M776">
+        <v>19.91</v>
+      </c>
+      <c r="N776" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="777" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A777" t="s">
+        <v>11</v>
+      </c>
+      <c r="B777" t="s">
+        <v>12</v>
+      </c>
+      <c r="C777" t="s">
+        <v>13</v>
+      </c>
+      <c r="D777" t="s">
+        <v>16</v>
+      </c>
+      <c r="E777" t="s">
+        <v>15</v>
+      </c>
+      <c r="F777" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G777" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H777">
+        <v>2</v>
+      </c>
+      <c r="I777">
+        <v>78</v>
+      </c>
+      <c r="J777" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K777">
+        <v>59.56</v>
+      </c>
+      <c r="L777">
+        <v>45.63</v>
+      </c>
+      <c r="M777">
+        <v>22.21</v>
+      </c>
+      <c r="N777" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="778" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A778" t="s">
+        <v>11</v>
+      </c>
+      <c r="B778" t="s">
+        <v>12</v>
+      </c>
+      <c r="C778" t="s">
+        <v>13</v>
+      </c>
+      <c r="D778" t="s">
+        <v>16</v>
+      </c>
+      <c r="E778" t="s">
+        <v>15</v>
+      </c>
+      <c r="F778" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G778" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H778">
+        <v>2</v>
+      </c>
+      <c r="I778">
+        <v>78</v>
+      </c>
+      <c r="J778" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K778">
+        <v>59.28</v>
+      </c>
+      <c r="L778">
+        <v>53.5</v>
+      </c>
+      <c r="M778">
+        <v>22.31</v>
+      </c>
+      <c r="N778" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="779" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A779" t="s">
+        <v>11</v>
+      </c>
+      <c r="B779" t="s">
+        <v>12</v>
+      </c>
+      <c r="C779" t="s">
+        <v>13</v>
+      </c>
+      <c r="D779" t="s">
+        <v>16</v>
+      </c>
+      <c r="E779" t="s">
+        <v>15</v>
+      </c>
+      <c r="F779" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G779" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H779">
+        <v>2</v>
+      </c>
+      <c r="I779">
+        <v>78</v>
+      </c>
+      <c r="J779" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K779">
+        <v>64.66</v>
+      </c>
+      <c r="L779">
+        <v>36.75</v>
+      </c>
+      <c r="M779">
+        <v>17.09</v>
+      </c>
+      <c r="N779" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="780" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A780" t="s">
+        <v>11</v>
+      </c>
+      <c r="B780" t="s">
+        <v>12</v>
+      </c>
+      <c r="C780" t="s">
+        <v>13</v>
+      </c>
+      <c r="D780" t="s">
+        <v>16</v>
+      </c>
+      <c r="E780" t="s">
+        <v>15</v>
+      </c>
+      <c r="F780" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G780" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H780">
+        <v>2</v>
+      </c>
+      <c r="I780">
+        <v>78</v>
+      </c>
+      <c r="J780" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K780">
+        <v>54.29</v>
+      </c>
+      <c r="L780">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="M780">
+        <v>22.19</v>
+      </c>
+      <c r="N780" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="781" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A781" t="s">
+        <v>11</v>
+      </c>
+      <c r="B781" t="s">
+        <v>12</v>
+      </c>
+      <c r="C781" t="s">
+        <v>13</v>
+      </c>
+      <c r="D781" t="s">
+        <v>16</v>
+      </c>
+      <c r="E781" t="s">
+        <v>15</v>
+      </c>
+      <c r="F781" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G781" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H781">
+        <v>2</v>
+      </c>
+      <c r="I781">
+        <v>78</v>
+      </c>
+      <c r="J781" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K781">
+        <v>75.38</v>
+      </c>
+      <c r="L781">
+        <v>44.7</v>
+      </c>
+      <c r="M781">
+        <v>15.73</v>
+      </c>
+      <c r="N781" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="782" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A782" t="s">
+        <v>11</v>
+      </c>
+      <c r="B782" t="s">
+        <v>12</v>
+      </c>
+      <c r="C782" t="s">
+        <v>13</v>
+      </c>
+      <c r="D782" t="s">
+        <v>14</v>
+      </c>
+      <c r="E782" t="s">
+        <v>15</v>
+      </c>
+      <c r="F782" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G782" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H782">
+        <v>7</v>
+      </c>
+      <c r="I782">
+        <v>77</v>
+      </c>
+      <c r="J782" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K782">
+        <v>75.19</v>
+      </c>
+      <c r="L782">
+        <v>49.91</v>
+      </c>
+      <c r="M782">
+        <v>20.94</v>
+      </c>
+      <c r="N782" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="783" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A783" t="s">
+        <v>11</v>
+      </c>
+      <c r="B783" t="s">
+        <v>12</v>
+      </c>
+      <c r="C783" t="s">
+        <v>13</v>
+      </c>
+      <c r="D783" t="s">
+        <v>14</v>
+      </c>
+      <c r="E783" t="s">
+        <v>15</v>
+      </c>
+      <c r="F783" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G783" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H783">
+        <v>7</v>
+      </c>
+      <c r="I783">
+        <v>77</v>
+      </c>
+      <c r="J783" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K783">
+        <v>43.46</v>
+      </c>
+      <c r="L783">
+        <v>39.49</v>
+      </c>
+      <c r="M783">
+        <v>15.65</v>
+      </c>
+      <c r="N783" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="784" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A784" t="s">
+        <v>11</v>
+      </c>
+      <c r="B784" t="s">
+        <v>12</v>
+      </c>
+      <c r="C784" t="s">
+        <v>13</v>
+      </c>
+      <c r="D784" t="s">
+        <v>14</v>
+      </c>
+      <c r="E784" t="s">
+        <v>15</v>
+      </c>
+      <c r="F784" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G784" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H784">
+        <v>7</v>
+      </c>
+      <c r="I784">
+        <v>77</v>
+      </c>
+      <c r="J784" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K784">
+        <v>51.81</v>
+      </c>
+      <c r="L784">
+        <v>38.35</v>
+      </c>
+      <c r="M784">
+        <v>13.89</v>
+      </c>
+      <c r="N784" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="785" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A785" t="s">
+        <v>11</v>
+      </c>
+      <c r="B785" t="s">
+        <v>12</v>
+      </c>
+      <c r="C785" t="s">
+        <v>13</v>
+      </c>
+      <c r="D785" t="s">
+        <v>14</v>
+      </c>
+      <c r="E785" t="s">
+        <v>15</v>
+      </c>
+      <c r="F785" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G785" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H785">
+        <v>7</v>
+      </c>
+      <c r="I785">
+        <v>77</v>
+      </c>
+      <c r="J785" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K785">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="L785">
+        <v>44.41</v>
+      </c>
+      <c r="M785">
+        <v>17.04</v>
+      </c>
+      <c r="N785" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="786" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A786" t="s">
+        <v>11</v>
+      </c>
+      <c r="B786" t="s">
+        <v>12</v>
+      </c>
+      <c r="C786" t="s">
+        <v>13</v>
+      </c>
+      <c r="D786" t="s">
+        <v>14</v>
+      </c>
+      <c r="E786" t="s">
+        <v>15</v>
+      </c>
+      <c r="F786" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G786" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H786">
+        <v>7</v>
+      </c>
+      <c r="I786">
+        <v>77</v>
+      </c>
+      <c r="J786" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K786">
+        <v>51.34</v>
+      </c>
+      <c r="L786">
+        <v>28.67</v>
+      </c>
+      <c r="M786">
+        <v>14.7</v>
+      </c>
+      <c r="N786" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="787" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A787" t="s">
+        <v>11</v>
+      </c>
+      <c r="B787" t="s">
+        <v>12</v>
+      </c>
+      <c r="C787" t="s">
+        <v>13</v>
+      </c>
+      <c r="D787" t="s">
+        <v>14</v>
+      </c>
+      <c r="E787" t="s">
+        <v>15</v>
+      </c>
+      <c r="F787" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G787" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H787">
+        <v>7</v>
+      </c>
+      <c r="I787">
+        <v>77</v>
+      </c>
+      <c r="J787" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K787">
+        <v>40.99</v>
+      </c>
+      <c r="L787">
+        <v>36.49</v>
+      </c>
+      <c r="M787">
+        <v>21.53</v>
+      </c>
+      <c r="N787" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="788" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A788" t="s">
+        <v>11</v>
+      </c>
+      <c r="B788" t="s">
+        <v>12</v>
+      </c>
+      <c r="C788" t="s">
+        <v>13</v>
+      </c>
+      <c r="D788" t="s">
+        <v>14</v>
+      </c>
+      <c r="E788" t="s">
+        <v>15</v>
+      </c>
+      <c r="F788" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G788" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H788">
+        <v>7</v>
+      </c>
+      <c r="I788">
+        <v>77</v>
+      </c>
+      <c r="J788" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K788">
+        <v>55.54</v>
+      </c>
+      <c r="L788">
+        <v>44.98</v>
+      </c>
+      <c r="M788">
+        <v>22</v>
+      </c>
+      <c r="N788" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="789" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A789" t="s">
+        <v>11</v>
+      </c>
+      <c r="B789" t="s">
+        <v>12</v>
+      </c>
+      <c r="C789" t="s">
+        <v>13</v>
+      </c>
+      <c r="D789" t="s">
+        <v>14</v>
+      </c>
+      <c r="E789" t="s">
+        <v>15</v>
+      </c>
+      <c r="F789" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G789" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H789">
+        <v>7</v>
+      </c>
+      <c r="I789">
+        <v>77</v>
+      </c>
+      <c r="J789" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K789">
+        <v>82.46</v>
+      </c>
+      <c r="L789">
+        <v>44.42</v>
+      </c>
+      <c r="M789">
+        <v>16.27</v>
+      </c>
+      <c r="N789" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="790" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A790" t="s">
+        <v>11</v>
+      </c>
+      <c r="B790" t="s">
+        <v>12</v>
+      </c>
+      <c r="C790" t="s">
+        <v>13</v>
+      </c>
+      <c r="D790" t="s">
+        <v>14</v>
+      </c>
+      <c r="E790" t="s">
+        <v>15</v>
+      </c>
+      <c r="F790" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G790" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H790">
+        <v>7</v>
+      </c>
+      <c r="I790">
+        <v>77</v>
+      </c>
+      <c r="J790" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K790">
+        <v>47.83</v>
+      </c>
+      <c r="L790">
+        <v>33.08</v>
+      </c>
+      <c r="M790">
+        <v>19.850000000000001</v>
+      </c>
+      <c r="N790" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="791" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A791" t="s">
+        <v>11</v>
+      </c>
+      <c r="B791" t="s">
+        <v>12</v>
+      </c>
+      <c r="C791" t="s">
+        <v>13</v>
+      </c>
+      <c r="D791" t="s">
+        <v>14</v>
+      </c>
+      <c r="E791" t="s">
+        <v>15</v>
+      </c>
+      <c r="F791" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G791" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H791">
+        <v>7</v>
+      </c>
+      <c r="I791">
+        <v>77</v>
+      </c>
+      <c r="J791" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K791">
+        <v>81.53</v>
+      </c>
+      <c r="L791">
+        <v>49.24</v>
+      </c>
+      <c r="M791">
+        <v>23.03</v>
+      </c>
+      <c r="N791" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="792" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A792" t="s">
+        <v>11</v>
+      </c>
+      <c r="B792" t="s">
+        <v>12</v>
+      </c>
+      <c r="C792" t="s">
+        <v>13</v>
+      </c>
+      <c r="D792" t="s">
+        <v>16</v>
+      </c>
+      <c r="E792" t="s">
+        <v>15</v>
+      </c>
+      <c r="F792" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G792" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H792">
+        <v>4</v>
+      </c>
+      <c r="I792">
+        <v>36</v>
+      </c>
+      <c r="J792" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K792">
+        <v>45.05</v>
+      </c>
+      <c r="L792">
+        <v>31.58</v>
+      </c>
+      <c r="M792">
+        <v>18.489999999999998</v>
+      </c>
+      <c r="N792" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="793" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A793" t="s">
+        <v>11</v>
+      </c>
+      <c r="B793" t="s">
+        <v>12</v>
+      </c>
+      <c r="C793" t="s">
+        <v>13</v>
+      </c>
+      <c r="D793" t="s">
+        <v>16</v>
+      </c>
+      <c r="E793" t="s">
+        <v>15</v>
+      </c>
+      <c r="F793" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G793" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H793">
+        <v>4</v>
+      </c>
+      <c r="I793">
+        <v>36</v>
+      </c>
+      <c r="J793" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K793">
+        <v>79.78</v>
+      </c>
+      <c r="L793">
+        <v>47.66</v>
+      </c>
+      <c r="M793">
+        <v>23.44</v>
+      </c>
+      <c r="N793" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="794" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A794" t="s">
+        <v>11</v>
+      </c>
+      <c r="B794" t="s">
+        <v>12</v>
+      </c>
+      <c r="C794" t="s">
+        <v>13</v>
+      </c>
+      <c r="D794" t="s">
+        <v>16</v>
+      </c>
+      <c r="E794" t="s">
+        <v>15</v>
+      </c>
+      <c r="F794" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G794" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H794">
+        <v>4</v>
+      </c>
+      <c r="I794">
+        <v>36</v>
+      </c>
+      <c r="J794" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K794">
+        <v>96.57</v>
+      </c>
+      <c r="L794">
+        <v>51.79</v>
+      </c>
+      <c r="M794">
+        <v>19.86</v>
+      </c>
+      <c r="N794" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="795" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A795" t="s">
+        <v>11</v>
+      </c>
+      <c r="B795" t="s">
+        <v>12</v>
+      </c>
+      <c r="C795" t="s">
+        <v>13</v>
+      </c>
+      <c r="D795" t="s">
+        <v>16</v>
+      </c>
+      <c r="E795" t="s">
+        <v>15</v>
+      </c>
+      <c r="F795" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G795" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H795">
+        <v>4</v>
+      </c>
+      <c r="I795">
+        <v>36</v>
+      </c>
+      <c r="J795" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K795">
+        <v>74.849999999999994</v>
+      </c>
+      <c r="L795">
+        <v>44.81</v>
+      </c>
+      <c r="M795">
+        <v>20.36</v>
+      </c>
+      <c r="N795" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="796" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A796" t="s">
+        <v>11</v>
+      </c>
+      <c r="B796" t="s">
+        <v>12</v>
+      </c>
+      <c r="C796" t="s">
+        <v>13</v>
+      </c>
+      <c r="D796" t="s">
+        <v>16</v>
+      </c>
+      <c r="E796" t="s">
+        <v>15</v>
+      </c>
+      <c r="F796" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G796" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H796">
+        <v>4</v>
+      </c>
+      <c r="I796">
+        <v>36</v>
+      </c>
+      <c r="J796" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K796">
+        <v>55.11</v>
+      </c>
+      <c r="L796">
+        <v>33.51</v>
+      </c>
+      <c r="M796">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="N796" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="797" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A797" t="s">
+        <v>11</v>
+      </c>
+      <c r="B797" t="s">
+        <v>12</v>
+      </c>
+      <c r="C797" t="s">
+        <v>13</v>
+      </c>
+      <c r="D797" t="s">
+        <v>16</v>
+      </c>
+      <c r="E797" t="s">
+        <v>15</v>
+      </c>
+      <c r="F797" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G797" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H797">
+        <v>4</v>
+      </c>
+      <c r="I797">
+        <v>36</v>
+      </c>
+      <c r="J797" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K797">
+        <v>59.99</v>
+      </c>
+      <c r="L797">
+        <v>36.47</v>
+      </c>
+      <c r="M797">
+        <v>25.26</v>
+      </c>
+      <c r="N797" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="798" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A798" t="s">
+        <v>11</v>
+      </c>
+      <c r="B798" t="s">
+        <v>12</v>
+      </c>
+      <c r="C798" t="s">
+        <v>13</v>
+      </c>
+      <c r="D798" t="s">
+        <v>16</v>
+      </c>
+      <c r="E798" t="s">
+        <v>15</v>
+      </c>
+      <c r="F798" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G798" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H798">
+        <v>4</v>
+      </c>
+      <c r="I798">
+        <v>36</v>
+      </c>
+      <c r="J798" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K798">
+        <v>54.92</v>
+      </c>
+      <c r="L798">
+        <v>38.130000000000003</v>
+      </c>
+      <c r="M798">
+        <v>20.83</v>
+      </c>
+      <c r="N798" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="799" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A799" t="s">
+        <v>11</v>
+      </c>
+      <c r="B799" t="s">
+        <v>12</v>
+      </c>
+      <c r="C799" t="s">
+        <v>13</v>
+      </c>
+      <c r="D799" t="s">
+        <v>16</v>
+      </c>
+      <c r="E799" t="s">
+        <v>15</v>
+      </c>
+      <c r="F799" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G799" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H799">
+        <v>4</v>
+      </c>
+      <c r="I799">
+        <v>36</v>
+      </c>
+      <c r="J799" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K799">
+        <v>63.26</v>
+      </c>
+      <c r="L799">
+        <v>59</v>
+      </c>
+      <c r="M799">
+        <v>18.7</v>
+      </c>
+      <c r="N799" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="800" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A800" t="s">
+        <v>11</v>
+      </c>
+      <c r="B800" t="s">
+        <v>12</v>
+      </c>
+      <c r="C800" t="s">
+        <v>13</v>
+      </c>
+      <c r="D800" t="s">
+        <v>16</v>
+      </c>
+      <c r="E800" t="s">
+        <v>15</v>
+      </c>
+      <c r="F800" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G800" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H800">
+        <v>4</v>
+      </c>
+      <c r="I800">
+        <v>36</v>
+      </c>
+      <c r="J800" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K800">
+        <v>71.849999999999994</v>
+      </c>
+      <c r="L800">
+        <v>36.1</v>
+      </c>
+      <c r="M800">
+        <v>20.74</v>
+      </c>
+      <c r="N800" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="801" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A801" t="s">
+        <v>11</v>
+      </c>
+      <c r="B801" t="s">
+        <v>12</v>
+      </c>
+      <c r="C801" t="s">
+        <v>13</v>
+      </c>
+      <c r="D801" t="s">
+        <v>16</v>
+      </c>
+      <c r="E801" t="s">
+        <v>15</v>
+      </c>
+      <c r="F801" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G801" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H801">
+        <v>4</v>
+      </c>
+      <c r="I801">
+        <v>36</v>
+      </c>
+      <c r="J801" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K801">
+        <v>78.790000000000006</v>
+      </c>
+      <c r="L801">
+        <v>53.46</v>
+      </c>
+      <c r="M801">
+        <v>25.24</v>
+      </c>
+      <c r="N801" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="802" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A802" t="s">
+        <v>11</v>
+      </c>
+      <c r="B802" t="s">
+        <v>12</v>
+      </c>
+      <c r="C802" t="s">
+        <v>13</v>
+      </c>
+      <c r="D802" t="s">
+        <v>14</v>
+      </c>
+      <c r="E802" t="s">
+        <v>15</v>
+      </c>
+      <c r="F802" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G802" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H802">
+        <v>9</v>
+      </c>
+      <c r="I802">
+        <v>95</v>
+      </c>
+      <c r="J802" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K802">
+        <v>49.02</v>
+      </c>
+      <c r="L802">
+        <v>28.29</v>
+      </c>
+      <c r="M802">
+        <v>14.55</v>
+      </c>
+      <c r="N802" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="803" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A803" t="s">
+        <v>11</v>
+      </c>
+      <c r="B803" t="s">
+        <v>12</v>
+      </c>
+      <c r="C803" t="s">
+        <v>13</v>
+      </c>
+      <c r="D803" t="s">
+        <v>14</v>
+      </c>
+      <c r="E803" t="s">
+        <v>15</v>
+      </c>
+      <c r="F803" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G803" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H803">
+        <v>9</v>
+      </c>
+      <c r="I803">
+        <v>95</v>
+      </c>
+      <c r="J803" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K803">
+        <v>76.39</v>
+      </c>
+      <c r="L803">
+        <v>50.64</v>
+      </c>
+      <c r="M803">
+        <v>15.99</v>
+      </c>
+      <c r="N803" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="804" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A804" t="s">
+        <v>11</v>
+      </c>
+      <c r="B804" t="s">
+        <v>12</v>
+      </c>
+      <c r="C804" t="s">
+        <v>13</v>
+      </c>
+      <c r="D804" t="s">
+        <v>14</v>
+      </c>
+      <c r="E804" t="s">
+        <v>15</v>
+      </c>
+      <c r="F804" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G804" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H804">
+        <v>9</v>
+      </c>
+      <c r="I804">
+        <v>95</v>
+      </c>
+      <c r="J804" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K804">
+        <v>62.09</v>
+      </c>
+      <c r="L804">
+        <v>53.7</v>
+      </c>
+      <c r="M804">
+        <v>22.77</v>
+      </c>
+      <c r="N804" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="805" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A805" t="s">
+        <v>11</v>
+      </c>
+      <c r="B805" t="s">
+        <v>12</v>
+      </c>
+      <c r="C805" t="s">
+        <v>13</v>
+      </c>
+      <c r="D805" t="s">
+        <v>14</v>
+      </c>
+      <c r="E805" t="s">
+        <v>15</v>
+      </c>
+      <c r="F805" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G805" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H805">
+        <v>9</v>
+      </c>
+      <c r="I805">
+        <v>95</v>
+      </c>
+      <c r="J805" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K805">
+        <v>62.72</v>
+      </c>
+      <c r="L805">
+        <v>43.52</v>
+      </c>
+      <c r="M805">
+        <v>19.62</v>
+      </c>
+      <c r="N805" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="806" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A806" t="s">
+        <v>11</v>
+      </c>
+      <c r="B806" t="s">
+        <v>12</v>
+      </c>
+      <c r="C806" t="s">
+        <v>13</v>
+      </c>
+      <c r="D806" t="s">
+        <v>14</v>
+      </c>
+      <c r="E806" t="s">
+        <v>15</v>
+      </c>
+      <c r="F806" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G806" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H806">
+        <v>9</v>
+      </c>
+      <c r="I806">
+        <v>95</v>
+      </c>
+      <c r="J806" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K806">
+        <v>84.76</v>
+      </c>
+      <c r="L806">
+        <v>50.06</v>
+      </c>
+      <c r="M806">
+        <v>20.69</v>
+      </c>
+      <c r="N806" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="807" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A807" t="s">
+        <v>11</v>
+      </c>
+      <c r="B807" t="s">
+        <v>12</v>
+      </c>
+      <c r="C807" t="s">
+        <v>13</v>
+      </c>
+      <c r="D807" t="s">
+        <v>14</v>
+      </c>
+      <c r="E807" t="s">
+        <v>15</v>
+      </c>
+      <c r="F807" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G807" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H807">
+        <v>9</v>
+      </c>
+      <c r="I807">
+        <v>95</v>
+      </c>
+      <c r="J807" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K807">
+        <v>78.31</v>
+      </c>
+      <c r="L807">
+        <v>47.8</v>
+      </c>
+      <c r="M807">
+        <v>24.97</v>
+      </c>
+      <c r="N807" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="808" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A808" t="s">
+        <v>11</v>
+      </c>
+      <c r="B808" t="s">
+        <v>12</v>
+      </c>
+      <c r="C808" t="s">
+        <v>13</v>
+      </c>
+      <c r="D808" t="s">
+        <v>14</v>
+      </c>
+      <c r="E808" t="s">
+        <v>15</v>
+      </c>
+      <c r="F808" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G808" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H808">
+        <v>9</v>
+      </c>
+      <c r="I808">
+        <v>95</v>
+      </c>
+      <c r="J808" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K808">
+        <v>57.16</v>
+      </c>
+      <c r="L808">
+        <v>45.75</v>
+      </c>
+      <c r="M808">
+        <v>20.8</v>
+      </c>
+      <c r="N808" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="809" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A809" t="s">
+        <v>11</v>
+      </c>
+      <c r="B809" t="s">
+        <v>12</v>
+      </c>
+      <c r="C809" t="s">
+        <v>13</v>
+      </c>
+      <c r="D809" t="s">
+        <v>14</v>
+      </c>
+      <c r="E809" t="s">
+        <v>15</v>
+      </c>
+      <c r="F809" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G809" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H809">
+        <v>9</v>
+      </c>
+      <c r="I809">
+        <v>95</v>
+      </c>
+      <c r="J809" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K809">
+        <v>56.08</v>
+      </c>
+      <c r="L809">
+        <v>59.39</v>
+      </c>
+      <c r="M809">
+        <v>19.79</v>
+      </c>
+      <c r="N809" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="810" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A810" t="s">
+        <v>11</v>
+      </c>
+      <c r="B810" t="s">
+        <v>12</v>
+      </c>
+      <c r="C810" t="s">
+        <v>13</v>
+      </c>
+      <c r="D810" t="s">
+        <v>14</v>
+      </c>
+      <c r="E810" t="s">
+        <v>15</v>
+      </c>
+      <c r="F810" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G810" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H810">
+        <v>9</v>
+      </c>
+      <c r="I810">
+        <v>95</v>
+      </c>
+      <c r="J810" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K810">
+        <v>64.39</v>
+      </c>
+      <c r="L810">
+        <v>50.7</v>
+      </c>
+      <c r="M810">
+        <v>21.62</v>
+      </c>
+      <c r="N810" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="811" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A811" t="s">
+        <v>11</v>
+      </c>
+      <c r="B811" t="s">
+        <v>12</v>
+      </c>
+      <c r="C811" t="s">
+        <v>13</v>
+      </c>
+      <c r="D811" t="s">
+        <v>14</v>
+      </c>
+      <c r="E811" t="s">
+        <v>15</v>
+      </c>
+      <c r="F811" s="1">
+        <v>45790</v>
+      </c>
+      <c r="G811" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H811">
+        <v>9</v>
+      </c>
+      <c r="I811">
+        <v>95</v>
+      </c>
+      <c r="J811" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K811">
+        <v>74.650000000000006</v>
+      </c>
+      <c r="L811">
+        <v>55.16</v>
+      </c>
+      <c r="M811">
+        <v>19.75</v>
+      </c>
+      <c r="N811" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>